<commit_message>
CAN lian tiao ji ben wan cheng
</commit_message>
<xml_diff>
--- a/Code/SDWE07C06Screen/MainScreen/VariateConfig.xlsx
+++ b/Code/SDWE07C06Screen/MainScreen/VariateConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9915"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6735"/>
   </bookViews>
   <sheets>
     <sheet name="全部变量" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="43">
   <si>
     <t>Image ID</t>
   </si>
@@ -65,52 +65,55 @@
     <t>卷帘门</t>
   </si>
   <si>
+    <t>0x0246</t>
+  </si>
+  <si>
+    <t>探测器</t>
+  </si>
+  <si>
+    <t>0x0230</t>
+  </si>
+  <si>
+    <t>0x0232</t>
+  </si>
+  <si>
+    <t>0x0234</t>
+  </si>
+  <si>
+    <t>三层路径</t>
+  </si>
+  <si>
+    <t>0x0244</t>
+  </si>
+  <si>
+    <t>0x0220</t>
+  </si>
+  <si>
+    <t>0x0222</t>
+  </si>
+  <si>
+    <t>0x0224</t>
+  </si>
+  <si>
+    <t>二层路径</t>
+  </si>
+  <si>
+    <t>0x0242</t>
+  </si>
+  <si>
+    <t>0x0210</t>
+  </si>
+  <si>
+    <t>0x0212</t>
+  </si>
+  <si>
+    <t>0x0214</t>
+  </si>
+  <si>
+    <t>一层路径</t>
+  </si>
+  <si>
     <t>0x0240</t>
-  </si>
-  <si>
-    <t>探测器</t>
-  </si>
-  <si>
-    <t>0x0230</t>
-  </si>
-  <si>
-    <t>0x0232</t>
-  </si>
-  <si>
-    <t>0x0234</t>
-  </si>
-  <si>
-    <t>三层路径</t>
-  </si>
-  <si>
-    <t>0x0244</t>
-  </si>
-  <si>
-    <t>0x0220</t>
-  </si>
-  <si>
-    <t>0x0222</t>
-  </si>
-  <si>
-    <t>0x0224</t>
-  </si>
-  <si>
-    <t>二层路径</t>
-  </si>
-  <si>
-    <t>0x0242</t>
-  </si>
-  <si>
-    <t>0x0210</t>
-  </si>
-  <si>
-    <t>0x0212</t>
-  </si>
-  <si>
-    <t>0x0214</t>
-  </si>
-  <si>
-    <t>一层路径</t>
   </si>
   <si>
     <t>IP地址</t>
@@ -525,10 +528,10 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -536,10 +539,10 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -547,10 +550,10 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -592,10 +595,10 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -637,13 +640,13 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -651,10 +654,10 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -662,10 +665,10 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -673,10 +676,10 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -752,10 +755,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -763,10 +766,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
@@ -774,10 +777,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -853,10 +856,10 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
@@ -864,10 +867,10 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
@@ -875,10 +878,10 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -940,7 +943,7 @@
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
         <v>29</v>
@@ -954,13 +957,13 @@
         <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
         <v>31</v>
-      </c>
-      <c r="D33" t="s">
-        <v>30</v>
       </c>
       <c r="E33" t="s">
         <v>6</v>
@@ -971,13 +974,13 @@
         <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" t="s">
         <v>33</v>
-      </c>
-      <c r="D34" t="s">
-        <v>32</v>
       </c>
       <c r="E34" t="s">
         <v>6</v>
@@ -988,13 +991,13 @@
         <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
         <v>35</v>
-      </c>
-      <c r="D35" t="s">
-        <v>34</v>
       </c>
       <c r="E35" t="s">
         <v>6</v>
@@ -1005,13 +1008,13 @@
         <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" t="s">
         <v>37</v>
-      </c>
-      <c r="D36" t="s">
-        <v>36</v>
       </c>
       <c r="E36" t="s">
         <v>6</v>
@@ -1022,13 +1025,13 @@
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" t="s">
         <v>39</v>
-      </c>
-      <c r="D37" t="s">
-        <v>38</v>
       </c>
       <c r="E37" t="s">
         <v>6</v>
@@ -1039,10 +1042,10 @@
         <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
@@ -1050,10 +1053,10 @@
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
@@ -1061,10 +1064,10 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
@@ -1072,10 +1075,10 @@
         <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1121,10 +1124,10 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -1132,10 +1135,10 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -1143,10 +1146,10 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -1154,10 +1157,10 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -1165,13 +1168,13 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -1179,10 +1182,10 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -1190,10 +1193,10 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -1201,10 +1204,10 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -1212,10 +1215,10 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -1223,10 +1226,10 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -1234,10 +1237,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -1245,10 +1248,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -1256,10 +1259,10 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -1267,10 +1270,10 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
@@ -1278,10 +1281,10 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
@@ -1289,10 +1292,10 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
@@ -1300,10 +1303,10 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
@@ -1311,10 +1314,10 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1632,7 +1635,7 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
         <v>29</v>
@@ -1646,13 +1649,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
         <v>31</v>
-      </c>
-      <c r="D19" t="s">
-        <v>30</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
@@ -1663,13 +1666,13 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
         <v>33</v>
-      </c>
-      <c r="D20" t="s">
-        <v>32</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
@@ -1680,13 +1683,13 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
         <v>35</v>
-      </c>
-      <c r="D21" t="s">
-        <v>34</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -1697,13 +1700,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
         <v>37</v>
-      </c>
-      <c r="D22" t="s">
-        <v>36</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -1714,13 +1717,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
         <v>39</v>
-      </c>
-      <c r="D23" t="s">
-        <v>38</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>

</xml_diff>